<commit_message>
mise à jour suivi
</commit_message>
<xml_diff>
--- a/point_sur_les_AUC_classif_deep_learning.xlsx
+++ b/point_sur_les_AUC_classif_deep_learning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ludo2\Documents\These\acousticpollinatordetection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F69A260-348F-4235-A5E5-E1BCEC10422C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{66E09F79-A0AF-44ED-932F-A0CA290E28BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5784" yWindow="264" windowWidth="11280" windowHeight="12096"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,47 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+  <si>
+    <t>Classifieur</t>
+  </si>
+  <si>
+    <t>nbepochs</t>
+  </si>
+  <si>
+    <t>batchsize</t>
+  </si>
+  <si>
+    <t>moteur</t>
+  </si>
+  <si>
+    <t>base_de_ref</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>sans_Homsap</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -65,8 +97,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,12 +416,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.81280640000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.89249849999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.88675090000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>75</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.87661239999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.89776999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.86260650000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.9019587</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>50</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.89508069999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>75</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.91835639999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.8850017</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test de differents classifieurs
</commit_message>
<xml_diff>
--- a/point_sur_les_AUC_classif_deep_learning.xlsx
+++ b/point_sur_les_AUC_classif_deep_learning.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ludo2\Documents\These\acousticpollinatordetection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ludovic Crochard\OneDrive\Documents\Acoustic-pollinator-detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{66E09F79-A0AF-44ED-932F-A0CA290E28BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>Classifieur</t>
   </si>
@@ -56,6 +55,75 @@
   </si>
   <si>
     <t>sans_Homsap</t>
+  </si>
+  <si>
+    <t>0.8427936</t>
+  </si>
+  <si>
+    <t>avec_Homsap</t>
+  </si>
+  <si>
+    <t>0.8805869</t>
+  </si>
+  <si>
+    <t>0.8707697</t>
+  </si>
+  <si>
+    <t>0.8857989</t>
+  </si>
+  <si>
+    <t>0.87121</t>
+  </si>
+  <si>
+    <t>0.7221667</t>
+  </si>
+  <si>
+    <t>0.8661407</t>
+  </si>
+  <si>
+    <t>0.8893093</t>
+  </si>
+  <si>
+    <t>0.8633324</t>
+  </si>
+  <si>
+    <t>0.9132991</t>
+  </si>
+  <si>
+    <t>0.8971631</t>
+  </si>
+  <si>
+    <t>0.900138</t>
+  </si>
+  <si>
+    <t>0.8999238</t>
+  </si>
+  <si>
+    <t>0.8870365</t>
+  </si>
+  <si>
+    <t>0.8701985</t>
+  </si>
+  <si>
+    <t>0.8816341</t>
+  </si>
+  <si>
+    <t>0.9098006</t>
+  </si>
+  <si>
+    <t>0.9162978</t>
+  </si>
+  <si>
+    <t>0.918523</t>
+  </si>
+  <si>
+    <t>0.9107287</t>
+  </si>
+  <si>
+    <t>0.8797658</t>
+  </si>
+  <si>
+    <t>0.9015303</t>
   </si>
 </sst>
 </file>
@@ -77,12 +145,42 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -97,11 +195,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,18 +526,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,204 +557,645 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>4</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3">
         <v>0.81280640000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>25</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>4</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3">
         <v>0.89249849999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>50</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>4</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3">
         <v>0.88675090000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>75</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3">
         <v>0.87661239999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>100</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>4</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3">
         <v>0.89776999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4">
         <v>10</v>
       </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="C7" s="4">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="5">
         <v>0.86260650000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4">
+        <v>8</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4">
         <v>25</v>
       </c>
-      <c r="C8">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="C9" s="4">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="5">
         <v>0.9019587</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>2</v>
+      </c>
+      <c r="B11" s="4">
+        <v>40</v>
+      </c>
+      <c r="C11" s="4">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4">
         <v>50</v>
       </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="C12" s="4">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="5">
         <v>0.89508069999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>2</v>
+      </c>
+      <c r="B13" s="4">
+        <v>60</v>
+      </c>
+      <c r="C13" s="4">
+        <v>8</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4">
+        <v>70</v>
+      </c>
+      <c r="C14" s="4">
+        <v>8</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4">
         <v>75</v>
       </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="C15" s="4">
+        <v>8</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="5">
         <v>0.91835639999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4">
+        <v>80</v>
+      </c>
+      <c r="C16" s="4">
+        <v>8</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4">
+        <v>90</v>
+      </c>
+      <c r="C17" s="4">
+        <v>8</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>2</v>
+      </c>
+      <c r="B18" s="4">
         <v>100</v>
       </c>
-      <c r="C11">
-        <v>8</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="C18" s="4">
+        <v>8</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="5">
         <v>0.8850017</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>5</v>
+      </c>
+      <c r="B19" s="8">
+        <v>10</v>
+      </c>
+      <c r="C19" s="8">
+        <v>8</v>
+      </c>
+      <c r="D19" s="8">
+        <v>2</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>5</v>
+      </c>
+      <c r="B20" s="8">
+        <v>25</v>
+      </c>
+      <c r="C20" s="8">
+        <v>8</v>
+      </c>
+      <c r="D20" s="8">
+        <v>2</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>5</v>
+      </c>
+      <c r="B21" s="8">
+        <v>50</v>
+      </c>
+      <c r="C21" s="8">
+        <v>8</v>
+      </c>
+      <c r="D21" s="8">
+        <v>2</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>5</v>
+      </c>
+      <c r="B22" s="8">
+        <v>75</v>
+      </c>
+      <c r="C22" s="8">
+        <v>8</v>
+      </c>
+      <c r="D22" s="8">
+        <v>2</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>5</v>
+      </c>
+      <c r="B23" s="8">
+        <v>100</v>
+      </c>
+      <c r="C23" s="8">
+        <v>8</v>
+      </c>
+      <c r="D23" s="8">
+        <v>2</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>3</v>
+      </c>
+      <c r="B24" s="10">
+        <v>10</v>
+      </c>
+      <c r="C24" s="10">
+        <v>2</v>
+      </c>
+      <c r="D24" s="10">
+        <v>2</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>3</v>
+      </c>
+      <c r="B25" s="10">
+        <v>25</v>
+      </c>
+      <c r="C25" s="10">
+        <v>2</v>
+      </c>
+      <c r="D25" s="10">
+        <v>2</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>3</v>
+      </c>
+      <c r="B26" s="10">
+        <v>50</v>
+      </c>
+      <c r="C26" s="10">
+        <v>2</v>
+      </c>
+      <c r="D26" s="10">
+        <v>2</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>3</v>
+      </c>
+      <c r="B27" s="10">
+        <v>75</v>
+      </c>
+      <c r="C27" s="10">
+        <v>2</v>
+      </c>
+      <c r="D27" s="10">
+        <v>2</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>3</v>
+      </c>
+      <c r="B28" s="10">
+        <v>100</v>
+      </c>
+      <c r="C28" s="10">
+        <v>2</v>
+      </c>
+      <c r="D28" s="10">
+        <v>2</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>4</v>
+      </c>
+      <c r="B29" s="6">
+        <v>10</v>
+      </c>
+      <c r="C29" s="6">
+        <v>6</v>
+      </c>
+      <c r="D29" s="6">
+        <v>2</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>4</v>
+      </c>
+      <c r="B30" s="6">
+        <v>25</v>
+      </c>
+      <c r="C30" s="6">
+        <v>6</v>
+      </c>
+      <c r="D30" s="6">
+        <v>2</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>4</v>
+      </c>
+      <c r="B31" s="6">
+        <v>50</v>
+      </c>
+      <c r="C31" s="6">
+        <v>6</v>
+      </c>
+      <c r="D31" s="6">
+        <v>2</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>4</v>
+      </c>
+      <c r="B32" s="6">
+        <v>75</v>
+      </c>
+      <c r="C32" s="6">
+        <v>6</v>
+      </c>
+      <c r="D32" s="6">
+        <v>2</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>4</v>
+      </c>
+      <c r="B33" s="6">
+        <v>100</v>
+      </c>
+      <c r="C33" s="6">
+        <v>6</v>
+      </c>
+      <c r="D33" s="6">
+        <v>2</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mise a jour suite aux premiers tests classif
</commit_message>
<xml_diff>
--- a/point_sur_les_AUC_classif_deep_learning.xlsx
+++ b/point_sur_les_AUC_classif_deep_learning.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="98">
   <si>
     <t>Classifieur</t>
   </si>
@@ -124,6 +125,210 @@
   </si>
   <si>
     <t>0.9015303</t>
+  </si>
+  <si>
+    <t>AUC avant suppression évènement trop court</t>
+  </si>
+  <si>
+    <t>AUC après supression évènement trop court</t>
+  </si>
+  <si>
+    <t>sans homsap</t>
+  </si>
+  <si>
+    <t>0.8745083</t>
+  </si>
+  <si>
+    <t>0.8901214</t>
+  </si>
+  <si>
+    <t>0.9222913</t>
+  </si>
+  <si>
+    <t>0.9462594</t>
+  </si>
+  <si>
+    <t>0.8981539</t>
+  </si>
+  <si>
+    <t>0.9179724</t>
+  </si>
+  <si>
+    <t>0.9044229</t>
+  </si>
+  <si>
+    <t>0.9278029</t>
+  </si>
+  <si>
+    <t>0.9137426</t>
+  </si>
+  <si>
+    <t>0.9369566</t>
+  </si>
+  <si>
+    <t>0.89336</t>
+  </si>
+  <si>
+    <t>0.912455</t>
+  </si>
+  <si>
+    <t>0.9166145</t>
+  </si>
+  <si>
+    <t>0.9354424</t>
+  </si>
+  <si>
+    <t>avec homsap</t>
+  </si>
+  <si>
+    <t>0.9286608</t>
+  </si>
+  <si>
+    <t>0.9478997</t>
+  </si>
+  <si>
+    <t>0.9131839</t>
+  </si>
+  <si>
+    <t>0.92934</t>
+  </si>
+  <si>
+    <t>0.9127928</t>
+  </si>
+  <si>
+    <t>0.9290991</t>
+  </si>
+  <si>
+    <t>0.9141449</t>
+  </si>
+  <si>
+    <t>0.9309</t>
+  </si>
+  <si>
+    <t>0.9191959</t>
+  </si>
+  <si>
+    <t>0.9366354</t>
+  </si>
+  <si>
+    <t>0.91524</t>
+  </si>
+  <si>
+    <t>0.9280552</t>
+  </si>
+  <si>
+    <t>0.9228165</t>
+  </si>
+  <si>
+    <t>0.9361995</t>
+  </si>
+  <si>
+    <t>0.9251855</t>
+  </si>
+  <si>
+    <t>0.9403634</t>
+  </si>
+  <si>
+    <t>0.9333542</t>
+  </si>
+  <si>
+    <t>0.9529239</t>
+  </si>
+  <si>
+    <t>0.893807</t>
+  </si>
+  <si>
+    <t>0.9138429</t>
+  </si>
+  <si>
+    <t>0.9177543</t>
+  </si>
+  <si>
+    <t>0.9358095</t>
+  </si>
+  <si>
+    <t>0.899819</t>
+  </si>
+  <si>
+    <t>0.9213563</t>
+  </si>
+  <si>
+    <t>0.9196317</t>
+  </si>
+  <si>
+    <t>0.9397669</t>
+  </si>
+  <si>
+    <t>0.9074513</t>
+  </si>
+  <si>
+    <t>0.9299135</t>
+  </si>
+  <si>
+    <t>0.9246044</t>
+  </si>
+  <si>
+    <t>0.9455367</t>
+  </si>
+  <si>
+    <t>0.9159217</t>
+  </si>
+  <si>
+    <t>0.9380578</t>
+  </si>
+  <si>
+    <t>0.9206486</t>
+  </si>
+  <si>
+    <t>0.9416022</t>
+  </si>
+  <si>
+    <t>0.9035401</t>
+  </si>
+  <si>
+    <t>0.9245452</t>
+  </si>
+  <si>
+    <t>0.9176873</t>
+  </si>
+  <si>
+    <t>0.9341577</t>
+  </si>
+  <si>
+    <t>0.9164469</t>
+  </si>
+  <si>
+    <t>0.9351557</t>
+  </si>
+  <si>
+    <t>0.925476</t>
+  </si>
+  <si>
+    <t>0.9454335</t>
+  </si>
+  <si>
+    <t>0.9091834</t>
+  </si>
+  <si>
+    <t>0.9293744</t>
+  </si>
+  <si>
+    <t>0.9125693</t>
+  </si>
+  <si>
+    <t>0.9341462</t>
+  </si>
+  <si>
+    <t>0.9173409</t>
+  </si>
+  <si>
+    <t>0.9393425</t>
+  </si>
+  <si>
+    <t>0.9187824</t>
+  </si>
+  <si>
+    <t>0.9396866</t>
   </si>
 </sst>
 </file>
@@ -145,7 +350,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +387,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -195,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -212,6 +435,9 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,4 +1428,783 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>50</v>
+      </c>
+      <c r="C3" s="4">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>75</v>
+      </c>
+      <c r="C4" s="4">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4">
+        <v>100</v>
+      </c>
+      <c r="C5" s="4">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4">
+        <v>125</v>
+      </c>
+      <c r="C6" s="4">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4">
+        <v>150</v>
+      </c>
+      <c r="C7" s="4">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4">
+        <v>175</v>
+      </c>
+      <c r="C8" s="4">
+        <v>8</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4">
+        <v>200</v>
+      </c>
+      <c r="C9" s="4">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>6</v>
+      </c>
+      <c r="B10" s="12">
+        <v>25</v>
+      </c>
+      <c r="C10" s="12">
+        <v>8</v>
+      </c>
+      <c r="D10" s="12">
+        <v>2</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>6</v>
+      </c>
+      <c r="B11" s="12">
+        <v>50</v>
+      </c>
+      <c r="C11" s="12">
+        <v>8</v>
+      </c>
+      <c r="D11" s="12">
+        <v>2</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="12">
+        <v>75</v>
+      </c>
+      <c r="C12" s="12">
+        <v>8</v>
+      </c>
+      <c r="D12" s="12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>6</v>
+      </c>
+      <c r="B13" s="12">
+        <v>100</v>
+      </c>
+      <c r="C13" s="12">
+        <v>8</v>
+      </c>
+      <c r="D13" s="12">
+        <v>2</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>6</v>
+      </c>
+      <c r="B14" s="12">
+        <v>125</v>
+      </c>
+      <c r="C14" s="12">
+        <v>8</v>
+      </c>
+      <c r="D14" s="12">
+        <v>2</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>6</v>
+      </c>
+      <c r="B15" s="12">
+        <v>150</v>
+      </c>
+      <c r="C15" s="12">
+        <v>8</v>
+      </c>
+      <c r="D15" s="12">
+        <v>2</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>6</v>
+      </c>
+      <c r="B16" s="12">
+        <v>175</v>
+      </c>
+      <c r="C16" s="12">
+        <v>8</v>
+      </c>
+      <c r="D16" s="12">
+        <v>2</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>6</v>
+      </c>
+      <c r="B17" s="12">
+        <v>200</v>
+      </c>
+      <c r="C17" s="12">
+        <v>8</v>
+      </c>
+      <c r="D17" s="12">
+        <v>2</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <v>3</v>
+      </c>
+      <c r="B18" s="13">
+        <v>25</v>
+      </c>
+      <c r="C18" s="13">
+        <v>16</v>
+      </c>
+      <c r="D18" s="13">
+        <v>2</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <v>3</v>
+      </c>
+      <c r="B19" s="13">
+        <v>50</v>
+      </c>
+      <c r="C19" s="13">
+        <v>16</v>
+      </c>
+      <c r="D19" s="13">
+        <v>2</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <v>3</v>
+      </c>
+      <c r="B20" s="13">
+        <v>75</v>
+      </c>
+      <c r="C20" s="13">
+        <v>16</v>
+      </c>
+      <c r="D20" s="13">
+        <v>2</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
+        <v>3</v>
+      </c>
+      <c r="B21" s="13">
+        <v>100</v>
+      </c>
+      <c r="C21" s="13">
+        <v>16</v>
+      </c>
+      <c r="D21" s="13">
+        <v>2</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>3</v>
+      </c>
+      <c r="B22" s="13">
+        <v>125</v>
+      </c>
+      <c r="C22" s="13">
+        <v>16</v>
+      </c>
+      <c r="D22" s="13">
+        <v>2</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
+        <v>3</v>
+      </c>
+      <c r="B23" s="13">
+        <v>150</v>
+      </c>
+      <c r="C23" s="13">
+        <v>16</v>
+      </c>
+      <c r="D23" s="13">
+        <v>2</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
+        <v>3</v>
+      </c>
+      <c r="B24" s="13">
+        <v>175</v>
+      </c>
+      <c r="C24" s="13">
+        <v>16</v>
+      </c>
+      <c r="D24" s="13">
+        <v>2</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>3</v>
+      </c>
+      <c r="B25" s="13">
+        <v>200</v>
+      </c>
+      <c r="C25" s="13">
+        <v>16</v>
+      </c>
+      <c r="D25" s="13">
+        <v>2</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <v>7</v>
+      </c>
+      <c r="B26" s="14">
+        <v>25</v>
+      </c>
+      <c r="C26" s="14">
+        <v>16</v>
+      </c>
+      <c r="D26" s="14">
+        <v>2</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>7</v>
+      </c>
+      <c r="B27" s="14">
+        <v>50</v>
+      </c>
+      <c r="C27" s="14">
+        <v>16</v>
+      </c>
+      <c r="D27" s="14">
+        <v>2</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>7</v>
+      </c>
+      <c r="B28" s="14">
+        <v>75</v>
+      </c>
+      <c r="C28" s="14">
+        <v>16</v>
+      </c>
+      <c r="D28" s="14">
+        <v>2</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>7</v>
+      </c>
+      <c r="B29" s="14">
+        <v>100</v>
+      </c>
+      <c r="C29" s="14">
+        <v>16</v>
+      </c>
+      <c r="D29" s="14">
+        <v>2</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>7</v>
+      </c>
+      <c r="B30" s="14">
+        <v>125</v>
+      </c>
+      <c r="C30" s="14">
+        <v>16</v>
+      </c>
+      <c r="D30" s="14">
+        <v>2</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>7</v>
+      </c>
+      <c r="B31" s="14">
+        <v>150</v>
+      </c>
+      <c r="C31" s="14">
+        <v>16</v>
+      </c>
+      <c r="D31" s="14">
+        <v>2</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>7</v>
+      </c>
+      <c r="B32" s="14">
+        <v>175</v>
+      </c>
+      <c r="C32" s="14">
+        <v>16</v>
+      </c>
+      <c r="D32" s="14">
+        <v>2</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>7</v>
+      </c>
+      <c r="B33" s="14">
+        <v>200</v>
+      </c>
+      <c r="C33" s="14">
+        <v>16</v>
+      </c>
+      <c r="D33" s="14">
+        <v>2</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>